<commit_message>
Merge Konflikte behoben und Vertrauensscore eingefügt
</commit_message>
<xml_diff>
--- a/nace_source_evaluation.xlsx
+++ b/nace_source_evaluation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1310,6 +1310,806 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Identifying the Human Rights Impacts of Palm Oil</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>A, B</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalyse für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Infrastructure"</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft &amp; Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>9</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Oil and Gas"</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>B, K</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>6</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Utilities and Waste Management"</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>D, K</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Strengthening Protection Against Trafficking in Persons in Federal and Corporate Supply Chains</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>5</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Human Rights Risks in Mining, A Baseline Study</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2022 List Of Goods Produced By Child Labor Or Forced Labor</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Die Achtung von Menschenrechten entlang globaler Wertschöpfungskette</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Global Estimates of Modern Slavery, Forced Labour and Forced Marriage</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Low Prices Drive Natural Rubber Producers Into Poverty</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Global Mercury Assessment 2018</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Sustainability and Circularity in the Textile Value Chain - A Global Roadmap</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Forced and Child Labour in the Cotton Industry</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Forced, child and trafficked labour in the cocoa industry</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Ermittlung von potentiell POP-haltigen Abfällen und Recyclingstoffen - Ableitung von Grenzwerten</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>6</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Kurzzeitige Chlorparafine (SCCP) Vorkommen, Verwendung und Rechtssetzung zu kurzketigen Chlorparaffinen in Produkten und Abfällen</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Hexabromocyclododecane</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>5</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Fairtrade Risk Map</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Typical Wastes Generated By Industry Sector</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Cocoa Barometer 2020</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalysen für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Human Rights Toolkit for Financial Institutions</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Global Dialogue Forum on Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft und Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Verité Commodity Atlas</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Business &amp; Human Rights Navigator</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>6</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Losing Ground, The Human Rights Impacts of Oil Palm Plantation Expansion in Indonesia</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>When We Lost the Forest, We Lost Everything: Oil Palm Plantations and Rights Violations in Indonesia</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>5</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2025-06-25 16:28:08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix: Risk-Scoring Fehler behoben
</commit_message>
<xml_diff>
--- a/nace_source_evaluation.xlsx
+++ b/nace_source_evaluation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Timestamp</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Risk_Score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,6 +489,7 @@
           <t>2025-06-25 12:56:16</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -509,6 +515,7 @@
           <t>2025-06-25 12:56:16</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -534,6 +541,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -559,6 +567,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -584,6 +593,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -609,6 +619,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -634,6 +645,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -659,6 +671,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -684,6 +697,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -709,6 +723,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -734,6 +749,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -759,6 +775,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -784,6 +801,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -809,6 +827,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -834,6 +853,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -859,6 +879,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -884,6 +905,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -909,6 +931,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -934,6 +957,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -959,6 +983,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -984,6 +1009,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1009,6 +1035,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1034,6 +1061,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1059,6 +1087,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1084,6 +1113,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1109,6 +1139,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1134,6 +1165,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1159,6 +1191,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1184,6 +1217,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1209,6 +1243,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1234,6 +1269,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1259,6 +1295,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1284,6 +1321,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1309,6 +1347,7 @@
           <t>2025-06-25 12:56:20</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1334,6 +1373,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1359,6 +1399,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1384,6 +1425,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1409,6 +1451,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1434,6 +1477,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1459,6 +1503,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1484,6 +1529,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1509,6 +1555,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1534,6 +1581,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1559,6 +1607,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1584,6 +1633,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1609,6 +1659,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1634,6 +1685,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1659,6 +1711,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1684,6 +1737,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1709,6 +1763,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1734,6 +1789,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1759,6 +1815,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1784,6 +1841,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1809,6 +1867,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1834,6 +1893,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1859,6 +1919,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1884,6 +1945,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1909,6 +1971,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1934,6 +1997,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1959,6 +2023,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1984,6 +2049,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2009,6 +2075,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2034,6 +2101,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2059,6 +2127,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2084,6 +2153,7 @@
           <t>2025-06-25 16:28:08</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2108,6 +2178,1799 @@
         <is>
           <t>2025-06-25 16:28:08</t>
         </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Identifying the Human Rights Impacts of Palm Oil</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalyse für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>A1, C10</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Infrastructure"</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>8</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>C14, C15</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft &amp; Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Oil and Gas"</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Utilities and Waste Management"</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>E38</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Strengthening Protection Against Trafficking in Persons in Federal and Corporate Supply Chains</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Human Rights Risks in Mining, A Baseline Study</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2022 List Of Goods Produced By Child Labor Or Forced Labor</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Die Achtung von Menschenrechten entlang globaler Wertschöpfungskette</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Global Estimates of Modern Slavery, Forced Labour and Forced Marriage</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>5</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Low Prices Drive Natural Rubber Producers Into Poverty</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Global Mercury Assessment 2018</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Sustainability and Circularity in the Textile Value Chain - A Global Roadmap</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>8</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Forced and Child Labour in the Cotton Industry</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Forced, child and trafficked labour in the cocoa industry</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>A1, C10</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Ermittlung von potentiell POP-haltigen Abfällen und Recyclingstoffen - Ableitung von Grenzwerten</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Kurzzeitige Chlorparafine (SCCP) Vorkommen, Verwendung und Rechtssetzung zu kurzketigen Chlorparaffinen in Produkten und Abfällen</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Hexabromocyclododecane</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Fairtrade Risk Map</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Typical Wastes Generated By Industry Sector</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Cocoa Barometer 2020</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>A1, C10</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalysen für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>A1, C10</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>5</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Human Rights Toolkit for Financial Institutions</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>C14, C15</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Global Dialogue Forum on Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>C14, C15</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft und Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Verité Commodity Atlas</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Business &amp; Human Rights Navigator</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Losing Ground, The Human Rights Impacts of Oil Palm Plantation Expansion in Indonesia</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>When We Lost the Forest, We Lost Everything: Oil Palm Plantations and Rights Violations in Indonesia</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:24:37</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Identifying the Human Rights Impacts of Palm Oil</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalyse für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>A1, C10</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Infrastructure"</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>8</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>C14, C15</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft &amp; Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Oil and Gas"</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Utilities and Waste Management"</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>E38</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Strengthening Protection Against Trafficking in Persons in Federal and Corporate Supply Chains</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Human Rights Risks in Mining, A Baseline Study</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2022 List Of Goods Produced By Child Labor Or Forced Labor</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Die Achtung von Menschenrechten entlang globaler Wertschöpfungskette</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Global Estimates of Modern Slavery, Forced Labour and Forced Marriage</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>5</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Low Prices Drive Natural Rubber Producers Into Poverty</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Global Mercury Assessment 2018</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Sustainability and Circularity in the Textile Value Chain - A Global Roadmap</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>8</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Forced and Child Labour in the Cotton Industry</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Forced, child and trafficked labour in the cocoa industry</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>A1, C10</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Ermittlung von potentiell POP-haltigen Abfällen und Recyclingstoffen - Ableitung von Grenzwerten</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Kurzzeitige Chlorparafine (SCCP) Vorkommen, Verwendung und Rechtssetzung zu kurzketigen Chlorparaffinen in Produkten und Abfällen</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Hexabromocyclododecane</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Fairtrade Risk Map</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Typical Wastes Generated By Industry Sector</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Cocoa Barometer 2020</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>A1, C10</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalysen für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>A1, C10</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>5</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Human Rights Toolkit for Financial Institutions</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>C14, C15</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Global Dialogue Forum on Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>C14, C15</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft und Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Verité Commodity Atlas</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Business &amp; Human Rights Navigator</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Losing Ground, The Human Rights Impacts of Oil Palm Plantation Expansion in Indonesia</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>When We Lost the Forest, We Lost Everything: Oil Palm Plantations and Rights Violations in Indonesia</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>2025-06-30 19:30:23</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KI für NACE-Bestimmung hinzugefügt und Codepflege
</commit_message>
<xml_diff>
--- a/nace_source_evaluation.xlsx
+++ b/nace_source_evaluation.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3973,6 +3973,1798 @@
         <v>7</v>
       </c>
     </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Identifying the Human Rights Impacts of Palm Oil</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalyse für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Infrastructure"</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>H50</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>8</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>C15</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft &amp; Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Oil and Gas"</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Utilities and Waste Management"</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>E38</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Strengthening Protection Against Trafficking in Persons in Federal and Corporate Supply Chains</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Human Rights Risks in Mining, A Baseline Study</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2022 List Of Goods Produced By Child Labor Or Forced Labor</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>C21</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Die Achtung von Menschenrechten entlang globaler Wertschöpfungskette</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Global Estimates of Modern Slavery, Forced Labour and Forced Marriage</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>5</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Low Prices Drive Natural Rubber Producers Into Poverty</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Global Mercury Assessment 2018</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Sustainability and Circularity in the Textile Value Chain - A Global Roadmap</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>8</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Forced and Child Labour in the Cotton Industry</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Forced, child and trafficked labour in the cocoa industry</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Ermittlung von potentiell POP-haltigen Abfällen und Recyclingstoffen - Ableitung von Grenzwerten</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Kurzzeitige Chlorparafine (SCCP) Vorkommen, Verwendung und Rechtssetzung zu kurzketigen Chlorparaffinen in Produkten und Abfällen</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Hexabromocyclododecane</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F151" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Fairtrade Risk Map</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Typical Wastes Generated By Industry Sector</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>C21</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Cocoa Barometer 2020</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalysen für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>5</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F155" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Human Rights Toolkit for Financial Institutions</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>C21</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>C15</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F157" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Global Dialogue Forum on Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>C15</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft und Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Verité Commodity Atlas</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F160" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Business &amp; Human Rights Navigator</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Losing Ground, The Human Rights Impacts of Oil Palm Plantation Expansion in Indonesia</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>When We Lost the Forest, We Lost Everything: Oil Palm Plantations and Rights Violations in Indonesia</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:27:14</t>
+        </is>
+      </c>
+      <c r="F163" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Identifying the Human Rights Impacts of Palm Oil</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalyse für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F165" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Infrastructure"</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>H50</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>8</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>C15</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft &amp; Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F168" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Oil and Gas"</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F169" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>UNEP FI Human Rights Guidance Tool for the Financial Sector "Utilities and Waste Management"</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>E38</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F170" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Strengthening Protection Against Trafficking in Persons in Federal and Corporate Supply Chains</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F171" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Human Rights Risks in Mining, A Baseline Study</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F172" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2022 List Of Goods Produced By Child Labor Or Forced Labor</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>C21</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F173" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Die Achtung von Menschenrechten entlang globaler Wertschöpfungskette</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F174" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Global Estimates of Modern Slavery, Forced Labour and Forced Marriage</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>5</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F175" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Low Prices Drive Natural Rubber Producers Into Poverty</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F176" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Global Mercury Assessment 2018</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F177" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Sustainability and Circularity in the Textile Value Chain - A Global Roadmap</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>8</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F178" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Forced and Child Labour in the Cotton Industry</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Forced, child and trafficked labour in the cocoa industry</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F180" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Ermittlung von potentiell POP-haltigen Abfällen und Recyclingstoffen - Ableitung von Grenzwerten</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F181" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Kurzzeitige Chlorparafine (SCCP) Vorkommen, Verwendung und Rechtssetzung zu kurzketigen Chlorparaffinen in Produkten und Abfällen</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F182" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Hexabromocyclododecane</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F183" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Fairtrade Risk Map</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F184" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Typical Wastes Generated By Industry Sector</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>C21</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F185" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Cocoa Barometer 2020</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F186" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Handlungsleitfaden zur Durchführung der Risikoanalysen für Kakao produzierende Länder</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>5</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F187" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Human Rights Toolkit for Financial Institutions</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>C21</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F188" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>C15</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F189" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Global Dialogue Forum on Wages and Working Hours in the Textiles, Clothing, Leather and Footwear Industries</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>C15</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F190" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Praxislotse Wirtschaft und Menschenrechte</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F191" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Verité Commodity Atlas</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Dr. Maria Schmidt</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F192" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Business &amp; Human Rights Navigator</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Prof. Dr. James Allen</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>D35</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F193" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Losing Ground, The Human Rights Impacts of Oil Palm Plantation Expansion in Indonesia</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Abdallah Reyati</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F194" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>When We Lost the Forest, We Lost Everything: Oil Palm Plantations and Rights Violations in Indonesia</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Lisa Müller</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>2025-07-03 03:56:32</t>
+        </is>
+      </c>
+      <c r="F195" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>